<commit_message>
Updated Gargoyles script and added readme.
</commit_message>
<xml_diff>
--- a/My Sets/Gargoyles (Mega Drive)/Gargoyles - Plan.xlsx
+++ b/My Sets/Gargoyles (Mega Drive)/Gargoyles - Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egrea\Dropbox\RetroArch\Achievements\Gargoyles\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\RetroArch\Achievements\Gargoyles\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="173">
   <si>
     <t>Description</t>
   </si>
@@ -253,21 +253,6 @@
     <t>Collect a hammer for temporary one-hit kills</t>
   </si>
   <si>
-    <t>Level 1 Speedrun</t>
-  </si>
-  <si>
-    <t>Level 2 Speedrun</t>
-  </si>
-  <si>
-    <t>Level 3 Speedrun</t>
-  </si>
-  <si>
-    <t>Level 4 Speedrun</t>
-  </si>
-  <si>
-    <t>Level 5 Speedrun</t>
-  </si>
-  <si>
     <t>Start of Level 1-1</t>
   </si>
   <si>
@@ -304,9 +289,6 @@
     <t>Fastest time to beat level 5 on normal+</t>
   </si>
   <si>
-    <t>Speedrun</t>
-  </si>
-  <si>
     <t>Fastest time to beat the game on normal+</t>
   </si>
   <si>
@@ -518,6 +500,69 @@
   </si>
   <si>
     <t>Complete the game without skipping levels</t>
+  </si>
+  <si>
+    <t>Any % Speedrun</t>
+  </si>
+  <si>
+    <t>Evil Awakens Speedrun</t>
+  </si>
+  <si>
+    <t>Siege of the Rookery Speedrun</t>
+  </si>
+  <si>
+    <t>Stone and Steel Speedrun</t>
+  </si>
+  <si>
+    <t>Subterranean Terror Speedrun</t>
+  </si>
+  <si>
+    <t>The Forge Speedrun</t>
+  </si>
+  <si>
+    <t>Fastest time to climb the lavafall on 5-4</t>
+  </si>
+  <si>
+    <t>Fastest time to run from the back of the train to the front on level 4-1</t>
+  </si>
+  <si>
+    <t>Fastest time to climb the ballista gauntlet on level 1-3</t>
+  </si>
+  <si>
+    <t>Fastest time to climb the rookery gauntlet to the vent switch on level 2-1</t>
+  </si>
+  <si>
+    <t>Fastest time to climb from the bottom of the Broadway Theater Group building to the top of the apartment building on level 3-2</t>
+  </si>
+  <si>
+    <t>Start in 1-3</t>
+  </si>
+  <si>
+    <t>Start in 2-1</t>
+  </si>
+  <si>
+    <t>Start in 3-2</t>
+  </si>
+  <si>
+    <t>Start in 4-1</t>
+  </si>
+  <si>
+    <t>Start in 5-4</t>
+  </si>
+  <si>
+    <t>Goal in 1-3</t>
+  </si>
+  <si>
+    <t>Goal in 2-1</t>
+  </si>
+  <si>
+    <t>Goal in 3-2</t>
+  </si>
+  <si>
+    <t>Goal in 4-1</t>
+  </si>
+  <si>
+    <t>Goal in 5-4</t>
   </si>
 </sst>
 </file>
@@ -889,8 +934,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I211"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1148,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H7" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1119,7 +1164,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>13</v>
@@ -1132,7 +1177,7 @@
         <v>12</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1161,7 +1206,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1177,7 +1222,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>13</v>
@@ -1190,7 +1235,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1219,7 +1264,7 @@
         <v>12</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1248,7 +1293,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H12" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1277,7 +1322,7 @@
         <v>37</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1293,7 +1338,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>34</v>
@@ -1306,7 +1351,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1322,7 +1367,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>12</v>
@@ -1335,14 +1380,14 @@
         <v>35</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H15" s="8" t="str">
         <f>IF(F15="Challenge",G15&amp;" on normal+ (see comments for map)",IF(F15="Easy",G15&amp;" on easy+",IF(F15="Normal",G15&amp;" on normal+",IF(F15="Hard",G15&amp;" on hard",""))))</f>
         <v>Climb the ballista gauntlet on level 1-3 in under 30 seconds on normal+ (see comments for map)</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1353,7 +1398,7 @@
         <v>35</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
@@ -1366,14 +1411,14 @@
         <v>35</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H16" s="8" t="str">
         <f>IF(F16="Challenge",G16&amp;" on normal+ (see comments for map)",IF(F16="Easy",G16&amp;" on easy+",IF(F16="Normal",G16&amp;" on normal+",IF(F16="Hard",G16&amp;" on hard",""))))</f>
         <v>Climb the rookery gauntlet to the vent switch on level 2-1 in under 25 seconds on normal+ (see comments for map)</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1384,7 +1429,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>12</v>
@@ -1397,14 +1442,14 @@
         <v>35</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Climb from the bottom of the Broadway Theater Group building to the top of the apartment building on level 3-2 in under 40 seconds on normal+ (see comments for map)</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1415,7 +1460,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>12</v>
@@ -1428,14 +1473,14 @@
         <v>35</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H18" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Run from the back of the train to the front on level 4-1 in under 60 seconds on normal+ (see comments for map)</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1446,7 +1491,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>12</v>
@@ -1459,14 +1504,14 @@
         <v>35</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H19" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Climb the lavafall on 5-4 in under 20 seconds on normal+ (see comments for map)</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1477,7 +1522,7 @@
         <v>58</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>9</v>
@@ -1506,7 +1551,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>17</v>
@@ -1535,7 +1580,7 @@
         <v>58</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>13</v>
@@ -1548,7 +1593,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H22" s="8" t="str">
         <f>IF(F22="Challenge",G22&amp;" on normal+ (see comments for map)",IF(F22="Easy",G22&amp;" on easy+",IF(F22="Normal",G22&amp;" on normal+",IF(F22="Hard",G22&amp;" on hard",""))))</f>
@@ -1564,7 +1609,7 @@
         <v>58</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>17</v>
@@ -1593,7 +1638,7 @@
         <v>58</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>10</v>
@@ -1606,7 +1651,7 @@
         <v>10</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H24" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1622,7 +1667,7 @@
         <v>58</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>17</v>
@@ -1651,7 +1696,7 @@
         <v>58</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>10</v>
@@ -1664,7 +1709,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H26" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1680,7 +1725,7 @@
         <v>58</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>10</v>
@@ -1693,7 +1738,7 @@
         <v>10</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H27" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1709,7 +1754,7 @@
         <v>58</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>10</v>
@@ -1722,7 +1767,7 @@
         <v>10</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H28" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1738,7 +1783,7 @@
         <v>58</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>17</v>
@@ -1767,7 +1812,7 @@
         <v>58</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>10</v>
@@ -1780,7 +1825,7 @@
         <v>10</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H30" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1796,7 +1841,7 @@
         <v>58</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>17</v>
@@ -1809,7 +1854,7 @@
         <v>10</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H31" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1825,7 +1870,7 @@
         <v>58</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>17</v>
@@ -1838,7 +1883,7 @@
         <v>10</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H32" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1854,7 +1899,7 @@
         <v>58</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>10</v>
@@ -1867,7 +1912,7 @@
         <v>10</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H33" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1883,7 +1928,7 @@
         <v>58</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>17</v>
@@ -1912,7 +1957,7 @@
         <v>58</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>17</v>
@@ -1941,7 +1986,7 @@
         <v>43</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>17</v>
@@ -1954,14 +1999,14 @@
         <v>37</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H36" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Knock out 25 Vikings in a single session on normal+</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1972,7 +2017,7 @@
         <v>43</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>12</v>
@@ -1992,7 +2037,7 @@
         <v>Knock out 50 Vikings in a single session on normal+</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2003,7 +2048,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>13</v>
@@ -2016,14 +2061,14 @@
         <v>37</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H38" s="8" t="str">
         <f t="shared" ref="H38" si="1">IF(F38="Challenge",G38&amp;" on normal+ (see comments for map)",IF(F38="Easy",G38&amp;" on easy+",IF(F38="Normal",G38&amp;" on normal+",IF(F38="Hard",G38&amp;" on hard",""))))</f>
         <v>Knock out 100 Vikings in a single session on normal+</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2034,7 +2079,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>13</v>
@@ -2047,14 +2092,14 @@
         <v>37</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H39" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Knock out 10 Valkyries in a single session on normal+</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2065,7 +2110,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>10</v>
@@ -2078,14 +2123,14 @@
         <v>37</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H40" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Knock out 25 Robots in a single session on normal+</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2096,7 +2141,7 @@
         <v>43</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>12</v>
@@ -2116,7 +2161,7 @@
         <v>Knock out 50 Robots in a single session on normal+</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2127,7 +2172,7 @@
         <v>43</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>13</v>
@@ -2140,14 +2185,14 @@
         <v>37</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H42" s="8" t="str">
         <f t="shared" ref="H42" si="2">IF(F42="Challenge",G42&amp;" on normal+ (see comments for map)",IF(F42="Easy",G42&amp;" on easy+",IF(F42="Normal",G42&amp;" on normal+",IF(F42="Hard",G42&amp;" on hard",""))))</f>
         <v>Knock out 100 Robots in a single session on normal+</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2158,7 +2203,7 @@
         <v>43</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>13</v>
@@ -2171,14 +2216,14 @@
         <v>37</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H43" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Knock out 10 Thor 3000s in a single session on normal+</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3654,7 +3699,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,114 +3742,114 @@
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G2" s="8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>74</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G3" s="8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G4" s="8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="G5" s="8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>72</v>
+      <c r="A6" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G6" s="8" t="b">
         <v>1</v>
@@ -3812,43 +3857,142 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>73</v>
+      <c r="A7" s="5" t="s">
+        <v>157</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G7" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="A11" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="A12" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="H12" s="8"/>
     </row>
   </sheetData>

</xml_diff>